<commit_message>
Grub: ausgemachte Sponsoren 1.GN-Sitzung
</commit_message>
<xml_diff>
--- a/2014/Sponsoring/Liste der Sponsoren.xlsx
+++ b/2014/Sponsoring/Liste der Sponsoren.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="125">
   <si>
     <t>Firma</t>
   </si>
@@ -386,6 +386,12 @@
   </si>
   <si>
     <t>Sponsoren von GN 2014</t>
+  </si>
+  <si>
+    <t>Lagerhaus Traunviertel</t>
+  </si>
+  <si>
+    <t>Bauplan-Hausbau Steyregg</t>
   </si>
 </sst>
 </file>
@@ -866,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FJ100"/>
+  <dimension ref="A1:FJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,7 +924,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="26">
-        <f>SUM(C8:C94)</f>
+        <f>SUM(C8:C95)</f>
         <v>0</v>
       </c>
       <c r="D4" s="24"/>
@@ -1124,7 +1130,7 @@
       <c r="FJ7" s="10"/>
     </row>
     <row r="8" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="A8" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="20" t="s">
@@ -1133,7 +1139,7 @@
       <c r="C8" s="14"/>
     </row>
     <row r="9" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -1143,7 +1149,7 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="A10" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B10" s="20" t="s">
@@ -1153,7 +1159,7 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -1164,7 +1170,7 @@
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="16" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -1175,17 +1181,17 @@
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>96</v>
+      <c r="A13" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B14" s="20" t="s">
@@ -1195,7 +1201,7 @@
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -1206,7 +1212,7 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:166" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="A16" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="20" t="s">
@@ -1217,7 +1223,7 @@
       <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="16" t="s">
         <v>51</v>
       </c>
       <c r="B17" s="20" t="s">
@@ -1228,256 +1234,236 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>97</v>
+      <c r="A18" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="C18" s="14"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>97</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="14"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="14"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B21" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="14"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="20" t="s">
+      <c r="C21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C21" s="14"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>69</v>
-      </c>
-      <c r="B22" s="20" t="s">
+      <c r="C22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
         <v>118</v>
-      </c>
-      <c r="C22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="C23" s="14"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="27"/>
+        <v>18</v>
+      </c>
+      <c r="C24" s="14"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="27"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="14"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="20" t="s">
+      <c r="C26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="14"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="B28" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="14"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="20" t="s">
+      <c r="C28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="20" t="s">
         <v>25</v>
-      </c>
-      <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="20" t="s">
-        <v>26</v>
       </c>
       <c r="C29" s="14"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="20"/>
+      <c r="B31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="15"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="14"/>
+      <c r="C31" s="15"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
-        <v>65</v>
+        <v>78</v>
       </c>
       <c r="B32" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="20"/>
+      <c r="B33" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="14"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B34" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="14"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B34" s="20" t="s">
+      <c r="B35" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B36" s="20" t="s">
         <v>32</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="H35" s="13"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>78</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>33</v>
       </c>
       <c r="C36" s="14"/>
       <c r="H36" s="13"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="14"/>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B38" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C37" s="14"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B39" s="20" t="s">
         <v>38</v>
-      </c>
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="20" t="s">
-        <v>116</v>
       </c>
       <c r="C39" s="14"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B40" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="C40" s="14"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="20" t="s">
         <v>71</v>
-      </c>
-      <c r="C40" s="14"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>60</v>
-      </c>
-      <c r="B41" s="20" t="s">
-        <v>57</v>
       </c>
       <c r="C41" s="14"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B42" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C42" s="14"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="C42" s="14"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="C43" s="14"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C44" s="14"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>67</v>
+        <v>85</v>
       </c>
       <c r="C45" s="14"/>
     </row>
@@ -1486,48 +1472,51 @@
         <v>78</v>
       </c>
       <c r="B46" s="20" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C46" s="14"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" s="14"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B48" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="14"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C48" s="14"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B49" s="20" t="s">
         <v>101</v>
-      </c>
-      <c r="C48" s="14"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>97</v>
-      </c>
-      <c r="B49" s="20" t="s">
-        <v>119</v>
       </c>
       <c r="C49" s="14"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>97</v>
       </c>
       <c r="B50" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C50" s="14"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="C50" s="14"/>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C51" s="7"/>
+      <c r="C51" s="14"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C52" s="7"/>
@@ -1675,6 +1664,9 @@
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C100" s="7"/>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>